<commit_message>
Revision 2 del JSON
</commit_message>
<xml_diff>
--- a/Documentacion/Testeo Funcional.xlsx
+++ b/Documentacion/Testeo Funcional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Scicchitano\Documents\Desarrollo HBL\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B233ED0-9EB1-4DF0-AC09-B0936C5B6204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C987A72C-72FB-4FCF-9005-343E0D369A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Testeo</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Testear el display LCD</t>
+  </si>
+  <si>
+    <t>Testear la lectura de ambos puertos seriales simultaneamente</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,9 +528,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>

</xml_diff>